<commit_message>
Add module ConsolidationOfResults to combine the results of two lines
</commit_message>
<xml_diff>
--- a/Результаты/выхДанные_Птицеплензавод.xlsx
+++ b/Результаты/выхДанные_Птицеплензавод.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Среднее значение отключаемой мощности</t>
   </si>
@@ -45,9 +45,6 @@
     <t>43,42,37,15,8,6,2</t>
   </si>
   <si>
-    <t xml:space="preserve">43,42,37,15,6,2 или 43,42,37,15,8,6 </t>
-  </si>
-  <si>
     <t>43,42,37,15,6</t>
   </si>
   <si>
@@ -55,6 +52,12 @@
   </si>
   <si>
     <t>37,15,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43,42,37,15,8,6 </t>
+  </si>
+  <si>
+    <t>15,6</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -162,12 +165,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,7 +759,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2560,7 +2565,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2597,7 +2602,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <f t="shared" ref="D2:D15" si="0">1-A2/$A$16</f>
         <v>0.78829609869956652</v>
       </c>
@@ -2611,7 +2616,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <f t="shared" si="0"/>
         <v>0.78825163943536736</v>
       </c>
@@ -2625,7 +2630,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <f t="shared" si="0"/>
         <v>0.78821829498721796</v>
       </c>
@@ -2639,7 +2644,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <f t="shared" si="0"/>
         <v>0.78815160609091917</v>
       </c>
@@ -2652,8 +2657,8 @@
       <c r="B6" s="8">
         <v>61</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="16">
+      <c r="C6" s="16"/>
+      <c r="D6" s="15">
         <f t="shared" si="0"/>
         <v>0.78807380237857061</v>
       </c>
@@ -2665,14 +2670,14 @@
       <c r="B7" s="6">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <f t="shared" si="0"/>
         <v>0.61401578303879067</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" ref="E7:E14" si="1">1-A7/A8</f>
         <v>3.5200311162971731E-2</v>
       </c>
@@ -2684,14 +2689,14 @@
       <c r="B8" s="6">
         <v>8</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <f t="shared" si="0"/>
         <v>0.59993331110370129</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="1"/>
         <v>3.4935785720030976E-2</v>
       </c>
@@ -2703,33 +2708,33 @@
       <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <f t="shared" si="0"/>
         <v>0.58545070579081915</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <f t="shared" si="1"/>
         <v>3.4881614697891083E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>3864.5</v>
       </c>
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="16">
+      <c r="C10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="15">
         <f t="shared" si="0"/>
         <v>0.57046793375569638</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <f t="shared" si="1"/>
         <v>3.370589853224315E-2</v>
       </c>
@@ -2741,14 +2746,14 @@
       <c r="B11" s="6">
         <v>5</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="16">
+      <c r="C11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
         <f t="shared" si="0"/>
         <v>0.55548516172057349</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <f t="shared" si="1"/>
         <v>8.0747483105778506E-2</v>
       </c>
@@ -2760,14 +2765,14 @@
       <c r="B12" s="6">
         <v>4</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="C12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="15">
         <f t="shared" si="0"/>
         <v>0.51643881293764582</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <f t="shared" si="1"/>
         <v>0.13927907252799432</v>
       </c>
@@ -2779,14 +2784,14 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="16">
+      <c r="C13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="15">
         <f t="shared" si="0"/>
         <v>0.43819050794709347</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <f t="shared" si="1"/>
         <v>0.14065183019092453</v>
       </c>
@@ -2798,14 +2803,14 @@
       <c r="B14" s="6">
         <v>2</v>
       </c>
-      <c r="C14" s="13">
-        <v>15.6</v>
-      </c>
-      <c r="D14" s="16">
+      <c r="C14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="15">
         <f t="shared" si="0"/>
         <v>0.34623763476714464</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <f t="shared" si="1"/>
         <v>0.17656199689210572</v>
       </c>
@@ -2817,14 +2822,14 @@
       <c r="B15" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="16">
         <v>15</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <f t="shared" si="0"/>
         <v>0.20605757474713793</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <f>1-A15/A16</f>
         <v>0.20605757474713793</v>
       </c>
@@ -2837,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <f>1-A16/$A$16</f>
         <v>0</v>
       </c>

</xml_diff>